<commit_message>
Ainda alguns errinhos na simulaçao
</commit_message>
<xml_diff>
--- a/Aula15/tabelinha.xlsx
+++ b/Aula15/tabelinha.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Descomp\DesignComp-Projeto2\Aula15\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Downloads\DesignComp-Projeto2\Aula15\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37ECEA78-F55A-4CB7-9D0E-B9ABAD24FF67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B860D9-B631-42CE-A31B-305A46D67238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12480" yWindow="6660" windowWidth="21600" windowHeight="11385" xr2:uid="{B56DCD25-DD30-4F59-AF24-F1D9751F2CAB}"/>
+    <workbookView xWindow="22800" yWindow="1650" windowWidth="17235" windowHeight="13830" xr2:uid="{B56DCD25-DD30-4F59-AF24-F1D9751F2CAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>LW</t>
   </si>
@@ -109,6 +109,27 @@
   </si>
   <si>
     <t>SUB</t>
+  </si>
+  <si>
+    <t>OPERAÇÃO</t>
+  </si>
+  <si>
+    <t>SOMA</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>USE O FUNCT</t>
+  </si>
+  <si>
+    <t>CODIGO</t>
+  </si>
+  <si>
+    <t>ANTIGO</t>
   </si>
 </sst>
 </file>
@@ -158,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -172,6 +193,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -191,7 +221,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -487,17 +517,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E197772-8A56-4E87-AD77-079DF697BC4B}">
-  <dimension ref="C2:N13"/>
+  <dimension ref="C2:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.42578125" customWidth="1"/>
     <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.85546875" customWidth="1"/>
@@ -767,6 +797,9 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
+      <c r="J9" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.25">
       <c r="D10" s="2"/>
@@ -779,18 +812,44 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
+      <c r="H11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.25">
       <c r="D12" s="2"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
+      <c r="H12" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="13" spans="3:14" x14ac:dyDescent="0.25">
       <c r="D13" s="2"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
+      <c r="H13" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="H14" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I14" s="1">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -799,6 +858,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <SharedWithUsers xmlns="286ddd33-a286-4f05-bbf4-221dca8b255d">
@@ -810,15 +878,6 @@
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1025,19 +1084,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{763A0F2F-7799-4727-AA2D-7D98108F00E5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A789EBDB-4E62-475A-A513-8515145C5351}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="286ddd33-a286-4f05-bbf4-221dca8b255d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{763A0F2F-7799-4727-AA2D-7D98108F00E5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>